<commit_message>
suppress previous existing XLSX
</commit_message>
<xml_diff>
--- a/TS_Themis VASILIKIOTIS.xlsx
+++ b/TS_Themis VASILIKIOTIS.xlsx
@@ -412,30 +412,6 @@
         <x:v>5</x:v>
       </x:c>
     </x:row>
-    <x:row r="4" spans="1:2">
-      <x:c r="A4" s="0" t="s">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="B4" s="0" t="s">
-        <x:v>1</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="5" spans="1:2">
-      <x:c r="A5" s="0" t="s">
-        <x:v>2</x:v>
-      </x:c>
-      <x:c r="B5" s="0" t="s">
-        <x:v>3</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="6" spans="1:2">
-      <x:c r="A6" s="0" t="s">
-        <x:v>4</x:v>
-      </x:c>
-      <x:c r="B6" s="0" t="s">
-        <x:v>5</x:v>
-      </x:c>
-    </x:row>
   </x:sheetData>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>

</xml_diff>